<commit_message>
Adding Lab Computer to git
</commit_message>
<xml_diff>
--- a/Acoustics Array Test Log.xlsx
+++ b/Acoustics Array Test Log.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Acoustics Testing Log" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +18,56 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Type of Test</t>
+  </si>
+  <si>
+    <t>Bats?</t>
+  </si>
+  <si>
+    <t>Ex. 16 June 23</t>
+  </si>
+  <si>
+    <t>Validation</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>2 mics not working, issues not diagnose; ai0 for each terminal not working</t>
+  </si>
+  <si>
+    <t>Operator</t>
+  </si>
+  <si>
+    <t>Bat Bot</t>
+  </si>
+  <si>
+    <t>Mic Status:</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +75,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,17 +118,135 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -331,12 +522,313 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AM3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="15.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="6"/>
+    <col min="4" max="4" width="19.7109375" style="6" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" style="6" customWidth="1"/>
+    <col min="7" max="7" width="5.5703125" style="6" customWidth="1"/>
+    <col min="8" max="39" width="4.7109375" style="6" customWidth="1"/>
+    <col min="40" max="16384" width="9.140625" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7">
+        <v>1</v>
+      </c>
+      <c r="H1" s="7">
+        <v>2</v>
+      </c>
+      <c r="I1" s="7">
+        <v>3</v>
+      </c>
+      <c r="J1" s="7">
+        <v>4</v>
+      </c>
+      <c r="K1" s="7">
+        <v>5</v>
+      </c>
+      <c r="L1" s="7">
+        <v>6</v>
+      </c>
+      <c r="M1" s="7">
+        <v>7</v>
+      </c>
+      <c r="N1" s="7">
+        <v>8</v>
+      </c>
+      <c r="O1" s="7">
+        <v>9</v>
+      </c>
+      <c r="P1" s="7">
+        <v>10</v>
+      </c>
+      <c r="Q1" s="7">
+        <v>11</v>
+      </c>
+      <c r="R1" s="7">
+        <v>12</v>
+      </c>
+      <c r="S1" s="7">
+        <v>13</v>
+      </c>
+      <c r="T1" s="7">
+        <v>14</v>
+      </c>
+      <c r="U1" s="7">
+        <v>15</v>
+      </c>
+      <c r="V1" s="7">
+        <v>16</v>
+      </c>
+      <c r="W1" s="7">
+        <v>17</v>
+      </c>
+      <c r="X1" s="7">
+        <v>18</v>
+      </c>
+      <c r="Y1" s="7">
+        <v>19</v>
+      </c>
+      <c r="Z1" s="7">
+        <v>20</v>
+      </c>
+      <c r="AA1" s="7">
+        <v>21</v>
+      </c>
+      <c r="AB1" s="7">
+        <v>22</v>
+      </c>
+      <c r="AC1" s="7">
+        <v>23</v>
+      </c>
+      <c r="AD1" s="7">
+        <v>24</v>
+      </c>
+      <c r="AE1" s="7">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="7">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="7">
+        <v>27</v>
+      </c>
+      <c r="AH1" s="7">
+        <v>28</v>
+      </c>
+      <c r="AI1" s="7">
+        <v>29</v>
+      </c>
+      <c r="AJ1" s="7">
+        <v>30</v>
+      </c>
+      <c r="AK1" s="7">
+        <v>31</v>
+      </c>
+      <c r="AL1" s="7">
+        <v>32</v>
+      </c>
+      <c r="AM1" s="12"/>
+    </row>
+    <row r="2" spans="1:39" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM2" s="13"/>
+    </row>
+    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
+      <c r="AA3" s="3"/>
+      <c r="AB3" s="3"/>
+      <c r="AC3" s="3"/>
+      <c r="AD3" s="3"/>
+      <c r="AE3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AG3" s="3"/>
+      <c r="AH3" s="3"/>
+      <c r="AI3" s="3"/>
+      <c r="AJ3" s="3"/>
+      <c r="AK3" s="3"/>
+      <c r="AL3" s="3"/>
+      <c r="AM3" s="13"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="G2:AM3">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>"Y"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"N"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G1:AL3">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating .git in the lab
</commit_message>
<xml_diff>
--- a/Acoustics Array Test Log.xlsx
+++ b/Acoustics Array Test Log.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C754A137-C2EF-431F-9F45-6DBFD725E260}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Acoustics Testing Log" sheetId="1" r:id="rId1"/>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="16">
   <si>
     <t>Date</t>
   </si>
@@ -61,12 +62,18 @@
   </si>
   <si>
     <t>Mic Status:</t>
+  </si>
+  <si>
+    <t>Sam Kramer</t>
+  </si>
+  <si>
+    <t>1 mic not working, working on diagnosis; ai0 not connected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,14 +144,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -172,30 +173,29 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -218,31 +218,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color rgb="FF9C6500"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -521,311 +501,383 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AM3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="R8" sqref="R8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="6" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="6" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="6"/>
-    <col min="4" max="4" width="19.7109375" style="6" customWidth="1"/>
-    <col min="5" max="5" width="40.5703125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" style="6" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" style="6" customWidth="1"/>
-    <col min="8" max="39" width="4.7109375" style="6" customWidth="1"/>
-    <col min="40" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="12.578125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="15.15625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="9.15625" style="4"/>
+    <col min="4" max="4" width="19.68359375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="40.578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="12.83984375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="5.578125" style="4" customWidth="1"/>
+    <col min="8" max="39" width="4.68359375" style="4" customWidth="1"/>
+    <col min="40" max="16384" width="9.15625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7">
+      <c r="F1" s="5"/>
+      <c r="G1" s="5">
         <v>1</v>
       </c>
-      <c r="H1" s="7">
+      <c r="H1" s="5">
         <v>2</v>
       </c>
-      <c r="I1" s="7">
+      <c r="I1" s="5">
         <v>3</v>
       </c>
-      <c r="J1" s="7">
+      <c r="J1" s="5">
         <v>4</v>
       </c>
-      <c r="K1" s="7">
+      <c r="K1" s="5">
         <v>5</v>
       </c>
-      <c r="L1" s="7">
+      <c r="L1" s="5">
         <v>6</v>
       </c>
-      <c r="M1" s="7">
+      <c r="M1" s="5">
         <v>7</v>
       </c>
-      <c r="N1" s="7">
-        <v>8</v>
-      </c>
-      <c r="O1" s="7">
+      <c r="N1" s="5">
+        <v>8</v>
+      </c>
+      <c r="O1" s="5">
         <v>9</v>
       </c>
-      <c r="P1" s="7">
+      <c r="P1" s="5">
         <v>10</v>
       </c>
-      <c r="Q1" s="7">
+      <c r="Q1" s="5">
         <v>11</v>
       </c>
-      <c r="R1" s="7">
+      <c r="R1" s="5">
         <v>12</v>
       </c>
-      <c r="S1" s="7">
+      <c r="S1" s="5">
         <v>13</v>
       </c>
-      <c r="T1" s="7">
+      <c r="T1" s="5">
         <v>14</v>
       </c>
-      <c r="U1" s="7">
+      <c r="U1" s="5">
         <v>15</v>
       </c>
-      <c r="V1" s="7">
+      <c r="V1" s="5">
         <v>16</v>
       </c>
-      <c r="W1" s="7">
+      <c r="W1" s="5">
         <v>17</v>
       </c>
-      <c r="X1" s="7">
+      <c r="X1" s="5">
         <v>18</v>
       </c>
-      <c r="Y1" s="7">
+      <c r="Y1" s="5">
         <v>19</v>
       </c>
-      <c r="Z1" s="7">
+      <c r="Z1" s="5">
         <v>20</v>
       </c>
-      <c r="AA1" s="7">
+      <c r="AA1" s="5">
         <v>21</v>
       </c>
-      <c r="AB1" s="7">
+      <c r="AB1" s="5">
         <v>22</v>
       </c>
-      <c r="AC1" s="7">
+      <c r="AC1" s="5">
         <v>23</v>
       </c>
-      <c r="AD1" s="7">
+      <c r="AD1" s="5">
         <v>24</v>
       </c>
-      <c r="AE1" s="7">
+      <c r="AE1" s="5">
         <v>25</v>
       </c>
-      <c r="AF1" s="7">
+      <c r="AF1" s="5">
         <v>26</v>
       </c>
-      <c r="AG1" s="7">
+      <c r="AG1" s="5">
         <v>27</v>
       </c>
-      <c r="AH1" s="7">
+      <c r="AH1" s="5">
         <v>28</v>
       </c>
-      <c r="AI1" s="7">
+      <c r="AI1" s="5">
         <v>29</v>
       </c>
-      <c r="AJ1" s="7">
+      <c r="AJ1" s="5">
         <v>30</v>
       </c>
-      <c r="AK1" s="7">
+      <c r="AK1" s="5">
         <v>31</v>
       </c>
-      <c r="AL1" s="7">
+      <c r="AL1" s="5">
         <v>32</v>
       </c>
-      <c r="AM1" s="12"/>
     </row>
-    <row r="2" spans="1:39" s="11" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:39" s="9" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="N2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" s="3" t="s">
+      <c r="H2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="P2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="W2" s="3" t="s">
+      <c r="Q2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Z2" s="3" t="s">
+      <c r="X2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AA2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="AF2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="AM2" s="13"/>
+      <c r="AF2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="3" spans="1:39" x14ac:dyDescent="0.25">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AJ3" s="3"/>
-      <c r="AK3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AM3" s="13"/>
+    <row r="3" spans="1:39" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="11">
+        <v>45097</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="2"/>
+      <c r="G3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="Z3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AC3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AD3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AE3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AG3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AH3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AI3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AJ3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AK3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AL3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="AM3" s="9"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="G1:AL3">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"NC"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G2:AM3">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"Y"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>"N"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="G1:AL3">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
-      <formula>"NC"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>